<commit_message>
update 3D數位內容與應用, add annotation in free.html
</commit_message>
<xml_diff>
--- a/media/Excel/109_data.xlsx
+++ b/media/Excel/109_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47376E28-6B6A-4F58-B2C0-8319F88E6EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC48BA3C-45FB-4663-9D7F-2619ABD94730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="必修" sheetId="1" r:id="rId1"/>
@@ -1554,10 +1554,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>3D 數位內容與應用</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>策略與管理的系統思維</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1695,10 +1691,6 @@
   </si>
   <si>
     <t>鄉村社會教育</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>咖啡學:消費與文化</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -2141,12 +2133,19 @@
   <si>
     <t>Linux 系統管理實務(一)$~$Linux 系統管理實務（一，入門）</t>
   </si>
+  <si>
+    <t>咖啡學：消費與文化</t>
+  </si>
+  <si>
+    <t>3D數位內容與應用</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2432,6 +2431,14 @@
     </font>
     <font>
       <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="微軟正黑體"/>
       <family val="2"/>
@@ -2796,7 +2803,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3032,6 +3039,15 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3112,12 +3128,6 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3423,201 +3433,201 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
-        <v>509</v>
-      </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="96"/>
+      <c r="A1" s="97" t="s">
+        <v>507</v>
+      </c>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="99"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="97"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="99"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="102"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="97"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="99"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="102"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="97"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="99"/>
+      <c r="A4" s="100"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="102"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="97"/>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="99"/>
+      <c r="A5" s="100"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="102"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="97"/>
-      <c r="B6" s="98"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="99"/>
+      <c r="A6" s="100"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="102"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="97"/>
-      <c r="B7" s="98"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="99"/>
+      <c r="A7" s="100"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="102"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="97"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="99"/>
+      <c r="A8" s="100"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="102"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="97"/>
-      <c r="B9" s="98"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="98"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="99"/>
+      <c r="A9" s="100"/>
+      <c r="B9" s="101"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="101"/>
+      <c r="K9" s="102"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="97"/>
-      <c r="B10" s="98"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98"/>
-      <c r="H10" s="98"/>
-      <c r="I10" s="98"/>
-      <c r="J10" s="98"/>
-      <c r="K10" s="99"/>
+      <c r="A10" s="100"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="101"/>
+      <c r="E10" s="101"/>
+      <c r="F10" s="101"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="101"/>
+      <c r="K10" s="102"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="97"/>
-      <c r="B11" s="98"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="99"/>
+      <c r="A11" s="100"/>
+      <c r="B11" s="101"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="101"/>
+      <c r="F11" s="101"/>
+      <c r="G11" s="101"/>
+      <c r="H11" s="101"/>
+      <c r="I11" s="101"/>
+      <c r="J11" s="101"/>
+      <c r="K11" s="102"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="97"/>
-      <c r="B12" s="98"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="98"/>
-      <c r="J12" s="98"/>
-      <c r="K12" s="99"/>
+      <c r="A12" s="100"/>
+      <c r="B12" s="101"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="101"/>
+      <c r="E12" s="101"/>
+      <c r="F12" s="101"/>
+      <c r="G12" s="101"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="101"/>
+      <c r="J12" s="101"/>
+      <c r="K12" s="102"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="97"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="98"/>
-      <c r="I13" s="98"/>
-      <c r="J13" s="98"/>
-      <c r="K13" s="99"/>
+      <c r="A13" s="100"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="101"/>
+      <c r="F13" s="101"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="101"/>
+      <c r="K13" s="102"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="97"/>
-      <c r="B14" s="98"/>
-      <c r="C14" s="98"/>
-      <c r="D14" s="98"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="98"/>
-      <c r="H14" s="98"/>
-      <c r="I14" s="98"/>
-      <c r="J14" s="98"/>
-      <c r="K14" s="99"/>
+      <c r="A14" s="100"/>
+      <c r="B14" s="101"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="101"/>
+      <c r="F14" s="101"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="101"/>
+      <c r="J14" s="101"/>
+      <c r="K14" s="102"/>
     </row>
     <row r="15" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="100"/>
-      <c r="B15" s="101"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="101"/>
-      <c r="I15" s="101"/>
-      <c r="J15" s="101"/>
-      <c r="K15" s="102"/>
+      <c r="A15" s="103"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="104"/>
+      <c r="G15" s="104"/>
+      <c r="H15" s="104"/>
+      <c r="I15" s="104"/>
+      <c r="J15" s="104"/>
+      <c r="K15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
@@ -3767,8 +3777,8 @@
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="112" t="s">
-        <v>564</v>
+      <c r="A23" s="85" t="s">
+        <v>562</v>
       </c>
       <c r="B23" s="15">
         <v>0.5</v>
@@ -3788,8 +3798,8 @@
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="112" t="s">
-        <v>565</v>
+      <c r="A24" s="85" t="s">
+        <v>563</v>
       </c>
       <c r="B24" s="15">
         <v>0.5</v>
@@ -3850,25 +3860,25 @@
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="85" t="s">
+      <c r="F27" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="86"/>
-      <c r="H27" s="86"/>
-      <c r="I27" s="86"/>
-      <c r="J27" s="87"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="90"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="91"/>
-      <c r="B28" s="92"/>
-      <c r="C28" s="92"/>
-      <c r="D28" s="93"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="89"/>
-      <c r="J28" s="90"/>
+      <c r="A28" s="94"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="96"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="92"/>
+      <c r="H28" s="92"/>
+      <c r="I28" s="92"/>
+      <c r="J28" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3889,7 +3899,7 @@
   </sheetPr>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -3909,7 +3919,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="16" customFormat="1" ht="51.6" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>1</v>
@@ -3921,7 +3931,7 @@
         <v>21</v>
       </c>
       <c r="E1" s="75" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F1" s="40" t="s">
         <v>1</v>
@@ -3933,7 +3943,7 @@
         <v>21</v>
       </c>
       <c r="I1" s="75" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J1" s="40" t="s">
         <v>1</v>
@@ -3999,7 +4009,7 @@
     </row>
     <row r="4" spans="1:12" s="16" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="41" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B4" s="41">
         <v>3</v>
@@ -4025,7 +4035,7 @@
     </row>
     <row r="5" spans="1:12" s="16" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B5" s="41">
         <v>3</v>
@@ -4077,7 +4087,7 @@
     </row>
     <row r="7" spans="1:12" s="16" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A7" s="48" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B7" s="40" t="s">
         <v>1</v>
@@ -4107,7 +4117,7 @@
     </row>
     <row r="8" spans="1:12" s="16" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="41" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B8" s="41">
         <v>3</v>
@@ -4159,7 +4169,7 @@
     </row>
     <row r="10" spans="1:12" s="16" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="41" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B10" s="41">
         <v>3</v>
@@ -4175,7 +4185,7 @@
       <c r="G10" s="41"/>
       <c r="H10" s="41"/>
       <c r="I10" s="41" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="J10" s="41">
         <v>3</v>
@@ -4192,8 +4202,8 @@
       </c>
       <c r="C11" s="41"/>
       <c r="D11" s="41"/>
-      <c r="E11" s="113" t="s">
-        <v>566</v>
+      <c r="E11" s="86" t="s">
+        <v>564</v>
       </c>
       <c r="F11" s="38">
         <v>3</v>
@@ -4201,7 +4211,7 @@
       <c r="G11" s="41"/>
       <c r="H11" s="41"/>
       <c r="I11" s="41" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="J11" s="41">
         <v>3</v>
@@ -4245,7 +4255,7 @@
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
       <c r="E13" s="41" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="F13" s="41">
         <v>3</v>
@@ -4253,7 +4263,7 @@
       <c r="G13" s="41"/>
       <c r="H13" s="41"/>
       <c r="I13" s="41" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="J13" s="41">
         <v>3</v>
@@ -4271,7 +4281,7 @@
       <c r="C14" s="41"/>
       <c r="D14" s="41"/>
       <c r="E14" s="39" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F14" s="41">
         <v>3</v>
@@ -4279,7 +4289,7 @@
       <c r="G14" s="41"/>
       <c r="H14" s="41"/>
       <c r="I14" s="39" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="J14" s="41">
         <v>3</v>
@@ -4371,8 +4381,8 @@
   </sheetPr>
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -4396,7 +4406,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -4464,7 +4474,7 @@
       <c r="K2" s="38"/>
       <c r="L2" s="38"/>
       <c r="M2" s="39" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="N2" s="38">
         <v>3</v>
@@ -4499,7 +4509,7 @@
       <c r="K3" s="38"/>
       <c r="L3" s="38"/>
       <c r="M3" s="38" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="N3" s="38">
         <v>3</v>
@@ -4536,7 +4546,7 @@
       <c r="K4" s="38"/>
       <c r="L4" s="38"/>
       <c r="M4" s="38" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="N4" s="38">
         <v>2</v>
@@ -4573,7 +4583,7 @@
       <c r="K5" s="38"/>
       <c r="L5" s="38"/>
       <c r="M5" s="84" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N5" s="84">
         <v>3</v>
@@ -4610,7 +4620,7 @@
       <c r="K6" s="38"/>
       <c r="L6" s="38"/>
       <c r="M6" s="84" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N6" s="84">
         <v>3</v>
@@ -4728,7 +4738,7 @@
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
       <c r="E10" s="38" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F10" s="38">
         <v>3</v>
@@ -4918,7 +4928,7 @@
     </row>
     <row r="16" spans="1:19" s="44" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="38" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B16" s="38">
         <v>3</v>
@@ -5083,7 +5093,7 @@
     </row>
     <row r="21" spans="1:19" s="44" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="38" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B21" s="38">
         <v>1</v>
@@ -5165,7 +5175,7 @@
       <c r="G23" s="38"/>
       <c r="H23" s="38"/>
       <c r="I23" s="38" t="s">
-        <v>448</v>
+        <v>566</v>
       </c>
       <c r="J23" s="38">
         <v>3</v>
@@ -5198,7 +5208,7 @@
       <c r="G24" s="38"/>
       <c r="H24" s="38"/>
       <c r="I24" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J24" s="38">
         <v>3</v>
@@ -5231,7 +5241,7 @@
       <c r="G25" s="38"/>
       <c r="H25" s="38"/>
       <c r="I25" s="38" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="J25" s="38">
         <v>3</v>
@@ -5264,7 +5274,7 @@
       <c r="G26" s="38"/>
       <c r="H26" s="38"/>
       <c r="I26" s="38" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="J26" s="38">
         <v>3</v>
@@ -5297,7 +5307,7 @@
       <c r="G27" s="38"/>
       <c r="H27" s="38"/>
       <c r="I27" s="38" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="J27" s="38">
         <v>3</v>
@@ -5330,7 +5340,7 @@
       <c r="G28" s="38"/>
       <c r="H28" s="38"/>
       <c r="I28" s="38" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J28" s="38">
         <v>3</v>
@@ -5363,7 +5373,7 @@
       <c r="G29" s="38"/>
       <c r="H29" s="38"/>
       <c r="I29" s="38" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="J29" s="38">
         <v>1</v>
@@ -5396,7 +5406,7 @@
       <c r="G30" s="38"/>
       <c r="H30" s="38"/>
       <c r="I30" s="38" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="J30" s="38">
         <v>1</v>
@@ -5676,7 +5686,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B5" s="31">
         <v>2</v>
@@ -5692,7 +5702,7 @@
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
       <c r="I5" s="25" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="J5" s="31">
         <v>3</v>
@@ -6228,7 +6238,7 @@
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="25" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F21" s="34">
         <v>3</v>
@@ -6618,7 +6628,7 @@
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
       <c r="M32" s="25" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="N32" s="31">
         <v>2</v>
@@ -6882,7 +6892,7 @@
       <c r="G40" s="20"/>
       <c r="H40" s="20"/>
       <c r="I40" s="69" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J40" s="61">
         <v>2</v>
@@ -6916,7 +6926,7 @@
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
       <c r="I41" s="63" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="J41" s="68">
         <v>3</v>
@@ -6950,7 +6960,7 @@
       <c r="G42" s="20"/>
       <c r="H42" s="20"/>
       <c r="I42" s="80" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="J42" s="81">
         <v>2</v>
@@ -6976,7 +6986,7 @@
       <c r="C43" s="20"/>
       <c r="D43" s="20"/>
       <c r="E43" s="63" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F43" s="64">
         <v>3</v>
@@ -7005,7 +7015,7 @@
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
       <c r="E44" s="67" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F44" s="64">
         <v>3</v>
@@ -7034,7 +7044,7 @@
       <c r="C45" s="20"/>
       <c r="D45" s="20"/>
       <c r="E45" s="67" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F45" s="66">
         <v>2</v>
@@ -7064,7 +7074,7 @@
       <c r="C46" s="26"/>
       <c r="D46" s="26"/>
       <c r="E46" s="67" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F46" s="66">
         <v>2</v>
@@ -7094,7 +7104,7 @@
       <c r="C47" s="26"/>
       <c r="D47" s="26"/>
       <c r="E47" s="67" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F47" s="66">
         <v>2</v>
@@ -7124,7 +7134,7 @@
       <c r="C48" s="26"/>
       <c r="D48" s="26"/>
       <c r="E48" s="67" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F48" s="72">
         <v>3</v>
@@ -7154,7 +7164,7 @@
       <c r="C49" s="26"/>
       <c r="D49" s="26"/>
       <c r="E49" s="63" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F49" s="72">
         <v>3</v>
@@ -7184,7 +7194,7 @@
       <c r="C50" s="26"/>
       <c r="D50" s="26"/>
       <c r="E50" s="80" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F50" s="83">
         <v>3</v>
@@ -7213,7 +7223,7 @@
       <c r="C51" s="26"/>
       <c r="D51" s="26"/>
       <c r="E51" s="80" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F51" s="83">
         <v>3</v>
@@ -7224,7 +7234,7 @@
       <c r="J51" s="65"/>
       <c r="K51" s="65"/>
       <c r="M51" s="63" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="N51" s="64">
         <v>2</v>
@@ -7243,7 +7253,7 @@
       <c r="C52" s="26"/>
       <c r="D52" s="26"/>
       <c r="E52" s="80" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F52" s="83">
         <v>2</v>
@@ -7254,7 +7264,7 @@
       <c r="J52" s="65"/>
       <c r="K52" s="65"/>
       <c r="M52" s="63" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N52" s="64">
         <v>2</v>
@@ -7273,7 +7283,7 @@
       <c r="C53" s="26"/>
       <c r="D53" s="26"/>
       <c r="E53" s="82" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F53" s="83">
         <v>2</v>
@@ -7284,7 +7294,7 @@
       <c r="J53" s="65"/>
       <c r="K53" s="65"/>
       <c r="M53" s="63" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="N53" s="64">
         <v>2</v>
@@ -7295,7 +7305,7 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A54" s="60" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B54" s="61">
         <v>3</v>
@@ -7303,7 +7313,7 @@
       <c r="C54" s="60"/>
       <c r="D54" s="60"/>
       <c r="M54" s="63" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="N54" s="64">
         <v>3</v>
@@ -7314,7 +7324,7 @@
     </row>
     <row r="55" spans="1:18" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="60" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B55" s="61">
         <v>2</v>
@@ -7325,7 +7335,7 @@
       <c r="F55" s="32"/>
       <c r="G55" s="28"/>
       <c r="M55" s="63" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="N55" s="72">
         <v>3</v>
@@ -7336,7 +7346,7 @@
     </row>
     <row r="56" spans="1:18" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="60" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B56" s="61">
         <v>3</v>
@@ -7344,17 +7354,17 @@
       <c r="C56" s="60"/>
       <c r="D56" s="60"/>
       <c r="E56"/>
-      <c r="F56" s="103" t="s">
-        <v>522</v>
-      </c>
-      <c r="G56" s="104"/>
-      <c r="H56" s="104"/>
-      <c r="I56" s="104"/>
-      <c r="J56" s="104"/>
-      <c r="K56" s="105"/>
+      <c r="F56" s="106" t="s">
+        <v>520</v>
+      </c>
+      <c r="G56" s="107"/>
+      <c r="H56" s="107"/>
+      <c r="I56" s="107"/>
+      <c r="J56" s="107"/>
+      <c r="K56" s="108"/>
       <c r="L56" s="28"/>
       <c r="M56" s="80" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="N56" s="79">
         <v>2</v>
@@ -7365,7 +7375,7 @@
     </row>
     <row r="57" spans="1:18" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="60" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B57" s="61">
         <v>2</v>
@@ -7373,15 +7383,15 @@
       <c r="C57" s="60"/>
       <c r="D57" s="60"/>
       <c r="E57"/>
-      <c r="F57" s="106"/>
-      <c r="G57" s="107"/>
-      <c r="H57" s="107"/>
-      <c r="I57" s="107"/>
-      <c r="J57" s="107"/>
-      <c r="K57" s="108"/>
+      <c r="F57" s="109"/>
+      <c r="G57" s="110"/>
+      <c r="H57" s="110"/>
+      <c r="I57" s="110"/>
+      <c r="J57" s="110"/>
+      <c r="K57" s="111"/>
       <c r="L57" s="28"/>
       <c r="M57" s="80" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="N57" s="79">
         <v>2</v>
@@ -7392,7 +7402,7 @@
     </row>
     <row r="58" spans="1:18" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="60" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B58" s="61">
         <v>2</v>
@@ -7400,15 +7410,15 @@
       <c r="C58" s="60"/>
       <c r="D58" s="60"/>
       <c r="E58"/>
-      <c r="F58" s="106"/>
-      <c r="G58" s="107"/>
-      <c r="H58" s="107"/>
-      <c r="I58" s="107"/>
-      <c r="J58" s="107"/>
-      <c r="K58" s="108"/>
+      <c r="F58" s="109"/>
+      <c r="G58" s="110"/>
+      <c r="H58" s="110"/>
+      <c r="I58" s="110"/>
+      <c r="J58" s="110"/>
+      <c r="K58" s="111"/>
       <c r="L58" s="28"/>
       <c r="M58" s="80" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="N58" s="79">
         <v>2</v>
@@ -7419,7 +7429,7 @@
     </row>
     <row r="59" spans="1:18" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="63" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B59" s="61">
         <v>3</v>
@@ -7427,15 +7437,15 @@
       <c r="C59" s="26"/>
       <c r="D59" s="62"/>
       <c r="E59"/>
-      <c r="F59" s="106"/>
-      <c r="G59" s="107"/>
-      <c r="H59" s="107"/>
-      <c r="I59" s="107"/>
-      <c r="J59" s="107"/>
-      <c r="K59" s="108"/>
+      <c r="F59" s="109"/>
+      <c r="G59" s="110"/>
+      <c r="H59" s="110"/>
+      <c r="I59" s="110"/>
+      <c r="J59" s="110"/>
+      <c r="K59" s="111"/>
       <c r="L59" s="28"/>
       <c r="M59" s="80" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="N59" s="79">
         <v>2</v>
@@ -7445,7 +7455,7 @@
     </row>
     <row r="60" spans="1:18" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="80" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B60" s="81">
         <v>3</v>
@@ -7453,15 +7463,15 @@
       <c r="C60" s="26"/>
       <c r="D60" s="62"/>
       <c r="E60"/>
-      <c r="F60" s="106"/>
-      <c r="G60" s="107"/>
-      <c r="H60" s="107"/>
-      <c r="I60" s="107"/>
-      <c r="J60" s="107"/>
-      <c r="K60" s="108"/>
+      <c r="F60" s="109"/>
+      <c r="G60" s="110"/>
+      <c r="H60" s="110"/>
+      <c r="I60" s="110"/>
+      <c r="J60" s="110"/>
+      <c r="K60" s="111"/>
       <c r="L60" s="28"/>
       <c r="M60" s="80" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="N60" s="79">
         <v>2</v>
@@ -7471,7 +7481,7 @@
     </row>
     <row r="61" spans="1:18" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="80" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B61" s="81">
         <v>3</v>
@@ -7479,15 +7489,15 @@
       <c r="C61" s="26"/>
       <c r="D61" s="62"/>
       <c r="E61"/>
-      <c r="F61" s="106"/>
-      <c r="G61" s="107"/>
-      <c r="H61" s="107"/>
-      <c r="I61" s="107"/>
-      <c r="J61" s="107"/>
-      <c r="K61" s="108"/>
+      <c r="F61" s="109"/>
+      <c r="G61" s="110"/>
+      <c r="H61" s="110"/>
+      <c r="I61" s="110"/>
+      <c r="J61" s="110"/>
+      <c r="K61" s="111"/>
       <c r="L61" s="28"/>
       <c r="M61" s="80" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="N61" s="79">
         <v>3</v>
@@ -7497,7 +7507,7 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A62" s="80" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B62" s="81">
         <v>3</v>
@@ -7505,18 +7515,18 @@
       <c r="C62" s="26"/>
       <c r="D62" s="62"/>
       <c r="E62"/>
-      <c r="F62" s="106"/>
-      <c r="G62" s="107"/>
-      <c r="H62" s="107"/>
-      <c r="I62" s="107"/>
-      <c r="J62" s="107"/>
-      <c r="K62" s="108"/>
+      <c r="F62" s="109"/>
+      <c r="G62" s="110"/>
+      <c r="H62" s="110"/>
+      <c r="I62" s="110"/>
+      <c r="J62" s="110"/>
+      <c r="K62" s="111"/>
       <c r="L62" s="28"/>
       <c r="N62" s="70"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A63" s="80" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B63" s="81">
         <v>3</v>
@@ -7524,19 +7534,19 @@
       <c r="C63" s="26"/>
       <c r="D63" s="62"/>
       <c r="E63"/>
-      <c r="F63" s="106"/>
-      <c r="G63" s="107"/>
-      <c r="H63" s="107"/>
-      <c r="I63" s="107"/>
-      <c r="J63" s="107"/>
-      <c r="K63" s="108"/>
+      <c r="F63" s="109"/>
+      <c r="G63" s="110"/>
+      <c r="H63" s="110"/>
+      <c r="I63" s="110"/>
+      <c r="J63" s="110"/>
+      <c r="K63" s="111"/>
       <c r="L63" s="28"/>
       <c r="M63"/>
       <c r="N63" s="70"/>
     </row>
     <row r="64" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="80" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B64" s="81">
         <v>2</v>
@@ -7544,19 +7554,19 @@
       <c r="C64" s="26"/>
       <c r="D64" s="62"/>
       <c r="E64"/>
-      <c r="F64" s="109"/>
-      <c r="G64" s="110"/>
-      <c r="H64" s="110"/>
-      <c r="I64" s="110"/>
-      <c r="J64" s="110"/>
-      <c r="K64" s="111"/>
+      <c r="F64" s="112"/>
+      <c r="G64" s="113"/>
+      <c r="H64" s="113"/>
+      <c r="I64" s="113"/>
+      <c r="J64" s="113"/>
+      <c r="K64" s="114"/>
       <c r="L64" s="28"/>
       <c r="M64"/>
       <c r="N64" s="70"/>
     </row>
     <row r="65" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A65" s="80" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B65" s="81">
         <v>1</v>
@@ -7573,7 +7583,7 @@
     </row>
     <row r="66" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A66" s="80" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B66" s="81">
         <v>3</v>
@@ -7590,7 +7600,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A67" s="80" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B67" s="81">
         <v>3</v>
@@ -7669,8 +7679,8 @@
   </sheetPr>
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView topLeftCell="G19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -7714,7 +7724,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="J1" s="24" t="s">
         <v>1</v>
@@ -7726,7 +7736,7 @@
         <v>3</v>
       </c>
       <c r="M1" s="73" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="N1" s="24" t="s">
         <v>1</v>
@@ -8345,7 +8355,7 @@
         <v>321</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="O19" s="20"/>
       <c r="P19" s="20"/>
@@ -8368,7 +8378,7 @@
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
       <c r="I20" s="20" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J20" s="20">
         <v>3</v>
@@ -8402,7 +8412,7 @@
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
       <c r="I21" s="20" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="J21" s="20">
         <v>3</v>
@@ -8470,7 +8480,7 @@
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
       <c r="I23" s="20" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J23" s="20">
         <v>3</v>
@@ -8504,7 +8514,7 @@
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
       <c r="I24" s="20" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J24" s="20">
         <v>2</v>
@@ -8538,7 +8548,7 @@
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
       <c r="I25" s="20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="J25" s="20">
         <v>2</v>
@@ -8572,7 +8582,7 @@
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="J26" s="20">
         <v>3</v>
@@ -8606,7 +8616,7 @@
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
       <c r="I27" s="20" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J27" s="20">
         <v>2</v>
@@ -8640,7 +8650,7 @@
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
       <c r="I28" s="20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J28" s="20">
         <v>3</v>
@@ -8674,7 +8684,7 @@
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
       <c r="I29" s="20" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="J29" s="20">
         <v>3</v>
@@ -8708,7 +8718,7 @@
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="J30" s="20">
         <v>3</v>
@@ -8742,7 +8752,7 @@
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
       <c r="I31" s="20" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J31" s="20">
         <v>3</v>
@@ -8776,7 +8786,7 @@
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
       <c r="I32" s="20" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="J32" s="20">
         <v>2</v>
@@ -8784,7 +8794,7 @@
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
       <c r="M32" s="37" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="N32" s="20">
         <v>3</v>
@@ -8802,7 +8812,7 @@
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
       <c r="E33" s="20" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F33" s="20">
         <v>3</v>
@@ -8810,7 +8820,7 @@
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
       <c r="I33" s="80" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J33" s="80">
         <v>3</v>
@@ -8844,7 +8854,7 @@
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
       <c r="I34" s="80" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J34" s="80">
         <v>2</v>
@@ -8852,7 +8862,7 @@
       <c r="K34" s="26"/>
       <c r="L34" s="26"/>
       <c r="M34" s="37" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N34" s="60">
         <v>3</v>
@@ -8878,15 +8888,15 @@
       <c r="G35" s="36"/>
       <c r="H35" s="36"/>
       <c r="I35" s="80" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J35" s="80">
         <v>3</v>
       </c>
       <c r="K35" s="26"/>
       <c r="L35" s="26"/>
-      <c r="M35" s="37" t="s">
-        <v>484</v>
+      <c r="M35" s="87" t="s">
+        <v>565</v>
       </c>
       <c r="N35" s="20">
         <v>2</v>
@@ -8912,7 +8922,7 @@
       <c r="G36" s="26"/>
       <c r="H36" s="26"/>
       <c r="I36" s="80" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="J36" s="80">
         <v>3</v>
@@ -8920,7 +8930,7 @@
       <c r="K36" s="26"/>
       <c r="L36" s="26"/>
       <c r="M36" s="37" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="N36" s="20">
         <v>3</v>
@@ -8930,7 +8940,7 @@
     </row>
     <row r="37" spans="1:16" ht="51.6" x14ac:dyDescent="0.5">
       <c r="A37" s="20" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B37" s="20">
         <v>3</v>
@@ -8946,7 +8956,7 @@
       <c r="G37" s="26"/>
       <c r="H37" s="26"/>
       <c r="I37" s="80" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="J37" s="80">
         <v>2</v>
@@ -8954,7 +8964,7 @@
       <c r="K37" s="26"/>
       <c r="L37" s="26"/>
       <c r="M37" s="37" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="N37" s="20">
         <v>3</v>
@@ -8964,7 +8974,7 @@
     </row>
     <row r="38" spans="1:16" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="20" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B38" s="20">
         <v>2</v>
@@ -8980,10 +8990,10 @@
       <c r="G38" s="26"/>
       <c r="H38" s="26"/>
       <c r="I38" s="19" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="J38" s="19" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="K38" s="24" t="s">
         <v>2</v>
@@ -8992,7 +9002,7 @@
         <v>3</v>
       </c>
       <c r="M38" s="80" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="N38" s="77">
         <v>2</v>
@@ -9002,7 +9012,7 @@
     </row>
     <row r="39" spans="1:16" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="20" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B39" s="20">
         <v>2</v>
@@ -9026,7 +9036,7 @@
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
       <c r="M39" s="80" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="N39" s="77">
         <v>2</v>
@@ -9036,7 +9046,7 @@
     </row>
     <row r="40" spans="1:16" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="76" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B40" s="77">
         <v>2</v>
@@ -9060,7 +9070,7 @@
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
       <c r="M40" s="80" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="N40" s="77">
         <v>2</v>
@@ -9070,7 +9080,7 @@
     </row>
     <row r="41" spans="1:16" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="78" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B41" s="77">
         <v>2</v>
@@ -9096,7 +9106,7 @@
     </row>
     <row r="42" spans="1:16" ht="51.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="78" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B42" s="77">
         <v>2</v>
@@ -9104,7 +9114,7 @@
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
       <c r="E42" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F42" s="20">
         <v>2</v>
@@ -9122,7 +9132,7 @@
     </row>
     <row r="43" spans="1:16" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="78" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B43" s="77">
         <v>3</v>
@@ -9130,7 +9140,7 @@
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
       <c r="E43" s="20" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F43" s="20">
         <v>2</v>
@@ -9148,7 +9158,7 @@
     </row>
     <row r="44" spans="1:16" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="78" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B44" s="77">
         <v>3</v>
@@ -9156,7 +9166,7 @@
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="76" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F44" s="77">
         <v>2</v>

</xml_diff>